<commit_message>
updated shapes for dataset 3
</commit_message>
<xml_diff>
--- a/03-Dataset3_Sessions/04-SHACL/Dataset3_Sessions-Shapes.xlsx
+++ b/03-Dataset3_Sessions/04-SHACL/Dataset3_Sessions-Shapes.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\00-Clients\EP\20-Repository\ep-graph-poc\03-Dataset3_Sessions\04-SHACL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F001D05-B08B-4623-91B5-29F39D0E89A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE59C65F-39EA-435C-9816-20E82B162714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="36540" windowHeight="18975" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14220" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="class-based shapes" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="121">
   <si>
     <t>URI du Graphe</t>
   </si>
@@ -253,9 +253,6 @@
     <t>xsd:date</t>
   </si>
   <si>
-    <t>rdf:plainLiteral</t>
-  </si>
-  <si>
     <t>sh:languageIn</t>
   </si>
   <si>
@@ -302,9 +299,6 @@
   </si>
   <si>
     <t>"^http://data.europarl.europa.eu/PlenarySession_[0-9][0-9][0-9][0-9][0-9][0-9][0-9][0-9]-[0-9][0-9][0-9][0-9][0-9][0-9][0-9][0-9]$"</t>
-  </si>
-  <si>
-    <t>"^http://data.europarl.europa.eu/PlenarySitting_[0-9][0-9][0-9][0-9][0-9][0-9]$"</t>
   </si>
   <si>
     <t>PlenarySession</t>
@@ -397,6 +391,15 @@
   </si>
   <si>
     <t>(subproperty of elidl:forms_part_of)</t>
+  </si>
+  <si>
+    <t>"^http://data.europarl.europa.eu/PlenarySitting_[0-9][0-9][0-9][0-9][0-9][0-9][0-9][0-9]$"</t>
+  </si>
+  <si>
+    <t>xsd:string</t>
+  </si>
+  <si>
+    <t>rdf:langString</t>
   </si>
 </sst>
 </file>
@@ -948,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK22"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView windowProtection="1" topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1013,10 +1016,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>77</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>78</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="2"/>
@@ -1110,17 +1113,17 @@
     </row>
     <row r="10" spans="1:11 1025:1025" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -1130,7 +1133,7 @@
         <v>18</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>48</v>
@@ -1141,17 +1144,17 @@
     </row>
     <row r="11" spans="1:11 1025:1025" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F11" s="1">
         <v>2</v>
@@ -1161,7 +1164,7 @@
         <v>18</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>48</v>
@@ -1240,9 +1243,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMN32"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1312,10 +1315,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>77</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>78</v>
       </c>
       <c r="F4"/>
       <c r="G4"/>
@@ -1412,7 +1415,7 @@
         <v>47</v>
       </c>
       <c r="T8" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AMM8"/>
       <c r="AMN8"/>
@@ -1446,7 +1449,7 @@
         <v>39</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>40</v>
@@ -1476,12 +1479,12 @@
         <v>46</v>
       </c>
       <c r="T9" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:20 1027:1028" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R10" s="20"/>
       <c r="T10" s="20"/>
@@ -1495,7 +1498,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
         <v>44</v>
@@ -1514,11 +1517,11 @@
         <v>45</v>
       </c>
       <c r="M11" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:20 1027:1028" ht="25.5" x14ac:dyDescent="0.2">
@@ -1527,13 +1530,13 @@
         <v>epsh:P12</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1555,13 +1558,13 @@
         <v>epsh:P13</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1582,19 +1585,19 @@
         <v>epsh:P14</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
         <v>82</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1</v>
-      </c>
-      <c r="J14" t="s">
-        <v>83</v>
       </c>
       <c r="L14" t="s">
         <v>18</v>
@@ -1612,7 +1615,7 @@
     </row>
     <row r="19" spans="1:20" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R19" s="20"/>
       <c r="T19" s="20"/>
@@ -1626,10 +1629,10 @@
         <v>69</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G20" s="1">
         <v>1</v>
@@ -1642,10 +1645,10 @@
         <v>45</v>
       </c>
       <c r="M20" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="51" x14ac:dyDescent="0.2">
@@ -1657,10 +1660,10 @@
         <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G21" s="1">
         <v>23</v>
@@ -1672,10 +1675,10 @@
         <v>45</v>
       </c>
       <c r="M21" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
@@ -1684,13 +1687,13 @@
         <v>epsh:P22</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G22" s="1">
         <v>1</v>
@@ -1711,13 +1714,13 @@
         <v>epsh:P23</v>
       </c>
       <c r="B23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G23" s="1">
         <v>1</v>
@@ -1726,7 +1729,7 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L23" t="s">
         <v>18</v>
@@ -1738,16 +1741,13 @@
         <v>epsh:P24</v>
       </c>
       <c r="B24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G24" s="1">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -1762,13 +1762,13 @@
         <v>epsh:P25</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G25" s="1">
         <v>1</v>
@@ -1786,13 +1786,13 @@
         <v>epsh:P26</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G26" s="1">
         <v>1</v>
@@ -1810,13 +1810,13 @@
         <v>epsh:P27</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G27" s="1">
         <v>1</v>
@@ -1834,13 +1834,13 @@
         <v>epsh:P28</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G28" s="1">
         <v>1</v>
@@ -1858,16 +1858,13 @@
         <v>epsh:P29</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G29" s="1">
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -1882,16 +1879,13 @@
         <v>epsh:P30</v>
       </c>
       <c r="B30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G30" s="1">
-        <v>1</v>
+        <v>110</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -1906,13 +1900,13 @@
         <v>epsh:P31</v>
       </c>
       <c r="B31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G31" s="1">
         <v>1</v>
@@ -1930,10 +1924,10 @@
         <v>epsh:P32</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L32" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Update SHACL specs of Dataset 3 with ep:hasParticipant to capture attendees
</commit_message>
<xml_diff>
--- a/03-Dataset3_Sessions/04-SHACL/Dataset3_Sessions-Shapes.xlsx
+++ b/03-Dataset3_Sessions/04-SHACL/Dataset3_Sessions-Shapes.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\00-Clients\EP\20-Repository\ep-graph-poc\03-Dataset3_Sessions\04-SHACL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE59C65F-39EA-435C-9816-20E82B162714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22387356-300C-49B2-909B-07B11BC8C137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14220" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20025" tabRatio="994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="class-based shapes" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="125">
   <si>
     <t>URI du Graphe</t>
   </si>
@@ -400,6 +400,18 @@
   </si>
   <si>
     <t>rdf:langString</t>
+  </si>
+  <si>
+    <t>ep:hasParticipant</t>
+  </si>
+  <si>
+    <t>subproperty of elidl:had_participant</t>
+  </si>
+  <si>
+    <t>ep:MEP</t>
+  </si>
+  <si>
+    <t>^http://data.europarl.europa.eu/MEP_[0-9][0-9][0-9][0-9]?[0-9]?[0-9]?$</t>
   </si>
 </sst>
 </file>
@@ -473,7 +485,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -498,6 +510,12 @@
         <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -512,7 +530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -566,6 +584,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1241,11 +1260,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMN32"/>
+  <dimension ref="A1:AMN33"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1622,7 +1641,7 @@
     </row>
     <row r="20" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
-        <f t="shared" ref="A20:A32" si="1">CONCATENATE("epsh:P",ROW(A20))</f>
+        <f t="shared" ref="A20:A33" si="1">CONCATENATE("epsh:P",ROW(A20))</f>
         <v>epsh:P20</v>
       </c>
       <c r="B20" t="s">
@@ -1931,6 +1950,30 @@
       </c>
       <c r="L32" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" t="str">
+        <f t="shared" si="1"/>
+        <v>epsh:P33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I33" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="L33" t="s">
+        <v>18</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update of all SHACL specifications to modify namespaces of URI
</commit_message>
<xml_diff>
--- a/03-Dataset3_Sessions/04-SHACL/Dataset3_Sessions-Shapes.xlsx
+++ b/03-Dataset3_Sessions/04-SHACL/Dataset3_Sessions-Shapes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="111">
   <si>
     <t xml:space="preserve">URI du Graphe</t>
   </si>
@@ -44,10 +44,10 @@
     <t xml:space="preserve">http://data.europarl.europa.eu/shapes#</t>
   </si>
   <si>
-    <t xml:space="preserve">elidl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://data.europa.eu/eli/eli-draft-legislation-ontology#</t>
+    <t xml:space="preserve">eponto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.europa.eu/ontology/ep#</t>
   </si>
   <si>
     <t xml:space="preserve">Cette feuille spécifie la liste de Shapes basées sur des classes</t>
@@ -98,7 +98,7 @@
     <t xml:space="preserve">sh:order^^xsd:integer</t>
   </si>
   <si>
-    <t xml:space="preserve">rdfs:comment@fr</t>
+    <t xml:space="preserve">rdfs:comment^^xsd:string</t>
   </si>
   <si>
     <t xml:space="preserve">sh:nodeKind</t>
@@ -119,225 +119,18 @@
     <t xml:space="preserve">sh:NodeShape</t>
   </si>
   <si>
-    <t xml:space="preserve">ep:PlenarySession</t>
+    <t xml:space="preserve">eponto:PlenarySession</t>
   </si>
   <si>
     <t xml:space="preserve">Plenary Session</t>
   </si>
   <si>
+    <t xml:space="preserve">eli/dl/iPlMeetingGroup/{starting date}-{ending date}
+Example :
+/eli/dl/iPlMeetingGroup/20191216-20191219</t>
+  </si>
+  <si>
     <t xml:space="preserve">sh:IRI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"^http://data.europarl.europa.eu/PlenarySession_[0-9][0-9][0-9][0-9][0-9][0-9][0-9][0-9]-[0-9][0-9][0-9][0-9][0-9][0-9][0-9][0-9]$"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(rdf:type)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epsh:PlenarySitting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep:PlenarySitting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plneary Sitting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"^http://data.europarl.europa.eu/PlenarySitting_[0-9][0-9][0-9][0-9][0-9][0-9]$"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cette feuille spécifie les contraintes sur les propriétés attachées à chaque Shape de la première feuille</t>
-  </si>
-  <si>
-    <t xml:space="preserve">URI de la contrainte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le prédicat ou path sur lequel la contrainte s’applique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La Shape à laquelle la contrainte est attachée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le niveau de sévérité de la contrainte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le nom de la contrainte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La description textuelle de la contrainte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La cardinalité minimum que le prédicat ou le path doit avoir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La cardinalité maximum que le prédicat ou le path doit avoir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Classe attendue comme valeur de la propriété, quand il n’y en a qu’une</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shape attendue comme valeur de la propriété</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Classes attendues comme valeur de la propriété, quand il y en a plusieurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le type de nœud que les valeurs devraient avoir (sh:IRI or sh:Literal)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pour les valeurs litérales, le type de données attendu pour les valeurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le type d'objet pour lequel les qualifiedMin ou MaxCount doivent être vérifié</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le nombre de fois minimum que le type indiqué dans sh:qualifiedValueShape doit être trouvé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le nombre de fois maximum que le type indiqué dans sh:qualifiedValueShape doit être trouvé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La liste des valeurs possibles pour la propriété, quand la liste de valeurs possible est petite et connue à l’avance.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La forme des URIs attendues comme valeur de la propriété, par exemple quand on s’attend à une URI GEONAMES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mettre à true dans le cas des skos:prefLabel pour indiquer qu'il ne faut qu'une seule valeur maximum par langue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La liste de code de langues autorisés pour cette valeur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^sh:property(separator=",")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:severity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:name@fr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:minCount^^xsd:integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:maxCount^^xsd:integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:node</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:or</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:datatype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:qualifiedValueShape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:qualifiedMinCount^^xsd:integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:qualifiedMaxCount^^xsd:integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:uniqueLang^^xsd:boolean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:languageIn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PlenarySession</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rdfs:label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:Violation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:Literal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rdf:plainLiteral</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plenary session from [0-9][0-9][0-9][0-9]-[0-9][0-9]-[0-9][0-9] to [0-9][0-9][0-9][0-9]-[0-9][0-9]-[0-9][0-9]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep:datePlenaryWeekBegin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activities[1].datePlenaryWeekBegin
-subproperty of elidl:activity_start_date)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xsd:date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep:datePlenaryWeekEnd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activities[3].datePlenaryWeekEnd
-subproperty of elidl:activity_end_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep:consistsOf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(subProperty of eli:consists_of)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PlenarySitting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">titles.short</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SESP [0-9][0-9][0-9][0-9]-[0-9][0-9]-[0-9][0-9]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skos:prefLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">titles.main (with language code)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">("hu" "et" "fi" "cs" "sk" "lt" "lv" "mt" "en" "da" "nl" "sv" "hr" "sl" "pl" "de" "ro" "it" "pt" "es" "fr" "ga" "el" "bg")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep:datePlenarySitting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datePlenarySitting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep:formsPartOf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(subproperty of elidl:forms_part_of)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep:hasAdoptedTextList</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activities[4].hasAdoptedTextList.relatedReference[0].uri</t>
   </si>
   <si>
     <r>
@@ -357,7 +150,57 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">http://data.europarl.europa.eu/reference/.*$</t>
+      <t xml:space="preserve">http://data.europarl.europa.eu/eli/dl/iPlMeetingGroup/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[0-9][0-9][0-9][0-9][0-9][0-9][0-9][0-9]-[0-9][0-9][0-9][0-9][0-9][0-9][0-9][0-9]$"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(rdf:type)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsh:PlenarySitting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:PlenarySitting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plneary Sitting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/eli/dl/iPlMeeting/{date}
+Example :
+/eli/dl/iPlMeeting/20191219</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">http://data.europarl.europa.eu/eli/dl/iPlMeeting/[0-9][0-9][0-9][0-9][0-9][0-9][0-9][0-9]$</t>
     </r>
     <r>
       <rPr>
@@ -370,58 +213,205 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">ep:hasAgenda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activities[5].hasAgenda.relatedReference[0].uri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep:hasAttendanceList</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activities[6].hasAttendanceList….</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep:hasCre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activities[7].hasCre…..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep:hasMinutes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activities[8]…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep:hasRollCallVotes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activities[9]….</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep:hasVoteResult</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activities[10]….</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep:hasLogisticMeeting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activities[11]….</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep:hasAnnex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep:hasParticipant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subproperty of elidl:had_participant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^http://data.europarl.europa.eu/MEP_[0-9][0-9][0-9][0-9]?[0-9]?[0-9]?$</t>
+    <t xml:space="preserve">Cette feuille spécifie les contraintes sur les propriétés attachées à chaque Shape de la première feuille</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URI de la contrainte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le prédicat ou path sur lequel la contrainte s’applique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La Shape à laquelle la contrainte est attachée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le niveau de sévérité de la contrainte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le nom de la contrainte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La description textuelle de la contrainte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La cardinalité minimum que le prédicat ou le path doit avoir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La cardinalité maximum que le prédicat ou le path doit avoir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classe attendue comme valeur de la propriété, quand il n’y en a qu’une</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shape attendue comme valeur de la propriété</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classes attendues comme valeur de la propriété, quand il y en a plusieurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le type de nœud que les valeurs devraient avoir (sh:IRI or sh:Literal)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pour les valeurs litérales, le type de données attendu pour les valeurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le type d'objet pour lequel les qualifiedMin ou MaxCount doivent être vérifié</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le nombre de fois minimum que le type indiqué dans sh:qualifiedValueShape doit être trouvé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le nombre de fois maximum que le type indiqué dans sh:qualifiedValueShape doit être trouvé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La liste des valeurs possibles pour la propriété, quand la liste de valeurs possible est petite et connue à l’avance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La forme des URIs attendues comme valeur de la propriété, par exemple quand on s’attend à une URI GEONAMES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mettre à true dans le cas des skos:prefLabel pour indiquer qu'il ne faut qu'une seule valeur maximum par langue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La liste de code de langues autorisés pour cette valeur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^sh:property(separator=",")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:severity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:name@fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:minCount^^xsd:integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:maxCount^^xsd:integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:node</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:datatype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:qualifiedValueShape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:qualifiedMinCount^^xsd:integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:qualifiedMaxCount^^xsd:integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:uniqueLang^^xsd:boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:languageIn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PlenarySession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdfs:label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:Violation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:Literal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xsd:string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plenary session from [0-9][0-9][0-9][0-9]-[0-9][0-9]-[0-9][0-9] to [0-9][0-9][0-9][0-9]-[0-9][0-9]-[0-9][0-9]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:datePlenaryWeekBegin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:datePlenaryWeekEnd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xsd:date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:consistsOf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PlenarySitting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SESP [0-9][0-9][0-9][0-9]-[0-9][0-9]-[0-9][0-9]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skos:prefLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdf:langString</t>
+  </si>
+  <si>
+    <t xml:space="preserve">("hu" "et" "fi" "cs" "sk" "lt" "lv" "mt" "en" "da" "nl" "sv" "hr" "sl" "pl" "de" "ro" "it" "pt" "es" "fr" "ga" "el" "bg")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:datePlenarySitting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:formsPartOf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:hasAdoptedTextList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/reference/.*$"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:hasAgenda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:hasAttendanceList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:hasCre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:hasMinutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:hasRollCallVotes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:hasVoteResult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:hasLogisticMeeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:hasAnnex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:hasParticipant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/person/MEP_[0-9][0-9][0-9][0-9]?[0-9]?[0-9]?$"</t>
   </si>
 </sst>
 </file>
@@ -431,7 +421,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -512,12 +502,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -595,6 +579,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -668,10 +656,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -755,11 +739,11 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.43359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.58"/>
@@ -768,7 +752,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="45.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.57"/>
@@ -782,130 +766,130 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="8" s="8" customFormat="true" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="8" s="9" customFormat="true" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>30</v>
       </c>
@@ -915,81 +899,85 @@
       <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="13"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="14" t="s">
         <v>35</v>
       </c>
+      <c r="I10" s="0" t="s">
+        <v>36</v>
+      </c>
       <c r="J10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="34.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="13"/>
+        <v>40</v>
+      </c>
+      <c r="D11" s="14"/>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="H11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G12" s="1"/>
-      <c r="I12" s="14"/>
+      <c r="I12" s="15"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G13" s="1"/>
-      <c r="I13" s="14"/>
+      <c r="I13" s="15"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="15"/>
+      <c r="D14" s="16"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="14"/>
+      <c r="I14" s="15"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,13 +1004,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="http://data.europarl.europa.eu/shapes"/>
-    <hyperlink ref="C2" r:id="rId2" display="http://data.europarl.europa.eu/"/>
-    <hyperlink ref="C3" r:id="rId3" display="http://data.europarl.europa.eu/shapes#"/>
-    <hyperlink ref="C4" r:id="rId4" display="http://data.europa.eu/eli/eli-draft-legislation-ontology#"/>
-    <hyperlink ref="E9" r:id="rId5" display="rdfs:label@fr"/>
-    <hyperlink ref="G9" r:id="rId6" display="rdfs:comment@fr"/>
-    <hyperlink ref="I10" r:id="rId7" display="&quot;^http://data.europarl.europa.eu/PlenarySession_[0-9][0-9][0-9][0-9][0-9][0-9][0-9][0-9]-[0-9][0-9][0-9][0-9][0-9][0-9][0-9][0-9]$&quot;"/>
-    <hyperlink ref="I11" r:id="rId8" display="&quot;^http://data.europarl.europa.eu/PlenarySitting_[0-9][0-9][0-9][0-9][0-9][0-9]$&quot;"/>
+    <hyperlink ref="E9" r:id="rId2" display="rdfs:label@fr"/>
+    <hyperlink ref="I10" r:id="rId3" display="http://data.europarl.europa.eu/eli/dl/iPlMeetingGroup/"/>
+    <hyperlink ref="I11" r:id="rId4" display="http://data.europarl.europa.eu/eli/dl/iPlMeeting/[0-9][0-9][0-9][0-9][0-9][0-9][0-9][0-9]$"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1041,28 +1025,28 @@
   </sheetPr>
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="R34" activeCellId="0" sqref="R34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="T33" activeCellId="0" sqref="T33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="40.42"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="34.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="26.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="41.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="34.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="28.14"/>
@@ -1077,200 +1061,200 @@
       </c>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="Q4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="3"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="7"/>
+      <c r="A6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" s="10" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" s="11" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="C8" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="D8" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="E8" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="F8" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="G8" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="H8" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="I8" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="J8" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="K8" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="L8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="O8" s="10" t="s">
+      <c r="M8" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="P8" s="10" t="s">
+      <c r="N8" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Q8" s="10" t="s">
+      <c r="O8" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="R8" s="10" t="s">
+      <c r="P8" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="S8" s="10" t="s">
+      <c r="Q8" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="T8" s="10" t="s">
+      <c r="R8" s="11" t="s">
         <v>62</v>
       </c>
+      <c r="S8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="T8" s="11" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="16" t="s">
+      <c r="B9" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="C9" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="D9" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="E9" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="F9" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="G9" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="H9" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="I9" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="L9" s="17" t="s">
+      <c r="J9" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="L9" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="N9" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="O9" s="17" t="s">
+      <c r="M9" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="P9" s="17" t="s">
+      <c r="N9" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="Q9" s="17" t="s">
+      <c r="O9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="R9" s="12" t="s">
+      <c r="P9" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q9" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="R9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="S9" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="T9" s="17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" s="19" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="s">
+      <c r="S9" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="R10" s="20"/>
-      <c r="T10" s="20"/>
+      <c r="T9" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" s="20" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="R10" s="21"/>
+      <c r="T10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="str">
@@ -1278,13 +1262,13 @@
         <v>epsh:P11</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E11" s="1" t="str">
         <f aca="false">CONCATENATE("Contraintes de ", B11, " sur un ", C11)</f>
@@ -1297,30 +1281,27 @@
         <v>1</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A12))</f>
         <v>epsh:P12</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="G12" s="1" t="n">
         <v>1</v>
       </c>
@@ -1328,14 +1309,14 @@
         <v>1</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="R12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+      <c r="R12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A13))</f>
         <v>epsh:P13</v>
@@ -1346,23 +1327,20 @@
       <c r="C13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="M13" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="G13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="M13" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A14))</f>
         <v>epsh:P14</v>
@@ -1373,49 +1351,43 @@
       <c r="C14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R17" s="4"/>
+    </row>
+    <row r="19" s="20" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="G14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="R14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R17" s="3"/>
-    </row>
-    <row r="19" s="19" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="R19" s="20"/>
-      <c r="T19" s="20"/>
-    </row>
-    <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R19" s="21"/>
+      <c r="T19" s="21"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A20))</f>
         <v>epsh:P20</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="G20" s="1" t="n">
         <v>1</v>
@@ -1423,30 +1395,27 @@
       <c r="H20" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J20" s="21"/>
+      <c r="J20" s="22"/>
       <c r="L20" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A21))</f>
         <v>epsh:P21</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="G21" s="1" t="n">
         <v>23</v>
@@ -1455,28 +1424,25 @@
         <v>23</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A22))</f>
         <v>epsh:P22</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>100</v>
+        <v>39</v>
       </c>
       <c r="G22" s="1" t="n">
         <v>1</v>
@@ -1485,25 +1451,22 @@
         <v>1</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A23))</f>
         <v>epsh:P23</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>102</v>
+        <v>39</v>
       </c>
       <c r="G23" s="1" t="n">
         <v>1</v>
@@ -1515,22 +1478,19 @@
         <v>30</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A24))</f>
         <v>epsh:P24</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>104</v>
+        <v>39</v>
       </c>
       <c r="G24" s="1" t="n">
         <v>1</v>
@@ -1539,25 +1499,22 @@
         <v>1</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+      <c r="R24" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A25))</f>
         <v>epsh:P25</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="G25" s="1" t="n">
         <v>1</v>
@@ -1566,10 +1523,10 @@
         <v>1</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>105</v>
+        <v>35</v>
+      </c>
+      <c r="R25" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1578,13 +1535,10 @@
         <v>epsh:P26</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="G26" s="1" t="n">
         <v>1</v>
@@ -1593,10 +1547,10 @@
         <v>1</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>105</v>
+        <v>35</v>
+      </c>
+      <c r="R26" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1605,13 +1559,10 @@
         <v>epsh:P27</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="G27" s="1" t="n">
         <v>1</v>
@@ -1620,10 +1571,10 @@
         <v>1</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>105</v>
+        <v>35</v>
+      </c>
+      <c r="R27" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1632,13 +1583,10 @@
         <v>epsh:P28</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="G28" s="1" t="n">
         <v>1</v>
@@ -1647,10 +1595,10 @@
         <v>1</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>105</v>
+        <v>35</v>
+      </c>
+      <c r="R28" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1659,13 +1607,10 @@
         <v>epsh:P29</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>115</v>
+        <v>39</v>
       </c>
       <c r="G29" s="1" t="n">
         <v>1</v>
@@ -1674,10 +1619,10 @@
         <v>1</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="R29" s="1" t="s">
-        <v>105</v>
+        <v>35</v>
+      </c>
+      <c r="R29" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,13 +1631,10 @@
         <v>epsh:P30</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>117</v>
+        <v>39</v>
       </c>
       <c r="G30" s="1" t="n">
         <v>1</v>
@@ -1701,10 +1643,10 @@
         <v>1</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>105</v>
+        <v>35</v>
+      </c>
+      <c r="R30" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1713,13 +1655,10 @@
         <v>epsh:P31</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>119</v>
+        <v>39</v>
       </c>
       <c r="G31" s="1" t="n">
         <v>1</v>
@@ -1728,10 +1667,10 @@
         <v>1</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>105</v>
+        <v>35</v>
+      </c>
+      <c r="R31" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,16 +1679,16 @@
         <v>epsh:P32</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>105</v>
+        <v>35</v>
+      </c>
+      <c r="R32" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1758,40 +1697,35 @@
         <v>epsh:P33</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
       <c r="G33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="R33" s="22" t="s">
-        <v>123</v>
+        <v>35</v>
+      </c>
+      <c r="R33" s="15" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="http://data.europarl.europa.eu/shapes"/>
-    <hyperlink ref="C2" r:id="rId2" display="http://data.europarl.europa.eu/"/>
-    <hyperlink ref="C3" r:id="rId3" display="http://data.europarl.europa.eu/shapes#"/>
-    <hyperlink ref="C4" r:id="rId4" display="http://data.europa.eu/eli/eli-draft-legislation-ontology#"/>
-    <hyperlink ref="E9" r:id="rId5" display="sh:name@fr"/>
-    <hyperlink ref="R24" r:id="rId6" display="http://data.europarl.europa.eu/reference/.*$"/>
-    <hyperlink ref="R25" r:id="rId7" display="http://data.europarl.europa.eu/reference/.*$"/>
-    <hyperlink ref="R26" r:id="rId8" display="http://data.europarl.europa.eu/reference/.*$"/>
-    <hyperlink ref="R27" r:id="rId9" display="http://data.europarl.europa.eu/reference/.*$"/>
-    <hyperlink ref="R28" r:id="rId10" display="http://data.europarl.europa.eu/reference/.*$"/>
-    <hyperlink ref="R29" r:id="rId11" display="http://data.europarl.europa.eu/reference/.*$"/>
-    <hyperlink ref="R30" r:id="rId12" display="http://data.europarl.europa.eu/reference/.*$"/>
-    <hyperlink ref="R31" r:id="rId13" display="http://data.europarl.europa.eu/reference/.*$"/>
-    <hyperlink ref="R32" r:id="rId14" display="http://data.europarl.europa.eu/reference/.*$"/>
+    <hyperlink ref="E9" r:id="rId2" display="sh:name@fr"/>
+    <hyperlink ref="R24" r:id="rId3" display="&quot;^http://data.europarl.europa.eu/reference/.*$&quot;"/>
+    <hyperlink ref="R25" r:id="rId4" display="&quot;^http://data.europarl.europa.eu/reference/.*$&quot;"/>
+    <hyperlink ref="R26" r:id="rId5" display="&quot;^http://data.europarl.europa.eu/reference/.*$&quot;"/>
+    <hyperlink ref="R27" r:id="rId6" display="&quot;^http://data.europarl.europa.eu/reference/.*$&quot;"/>
+    <hyperlink ref="R28" r:id="rId7" display="&quot;^http://data.europarl.europa.eu/reference/.*$&quot;"/>
+    <hyperlink ref="R29" r:id="rId8" display="&quot;^http://data.europarl.europa.eu/reference/.*$&quot;"/>
+    <hyperlink ref="R30" r:id="rId9" display="&quot;^http://data.europarl.europa.eu/reference/.*$&quot;"/>
+    <hyperlink ref="R31" r:id="rId10" display="&quot;^http://data.europarl.europa.eu/reference/.*$&quot;"/>
+    <hyperlink ref="R32" r:id="rId11" display="&quot;^http://data.europarl.europa.eu/reference/.*$&quot;"/>
+    <hyperlink ref="R33" r:id="rId12" display="&quot;^http://data.europarl.europa.eu/person/MEP_[0-9][0-9][0-9][0-9]?[0-9]?[0-9]?$&quot;"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Remove cardinality constraint on hasParticipant
</commit_message>
<xml_diff>
--- a/03-Dataset3_Sessions/04-SHACL/Dataset3_Sessions-Shapes.xlsx
+++ b/03-Dataset3_Sessions/04-SHACL/Dataset3_Sessions-Shapes.xlsx
@@ -970,7 +970,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+      <selection pane="bottomLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1635,9 +1635,6 @@
       <c r="C33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G33" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="L33" s="0" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Update URI pattern for references to documents
</commit_message>
<xml_diff>
--- a/03-Dataset3_Sessions/04-SHACL/Dataset3_Sessions-Shapes.xlsx
+++ b/03-Dataset3_Sessions/04-SHACL/Dataset3_Sessions-Shapes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="112">
   <si>
     <t xml:space="preserve">URI du Graphe</t>
   </si>
@@ -327,10 +327,67 @@
     <t xml:space="preserve">eponto:hasAdoptedTextList</t>
   </si>
   <si>
-    <t xml:space="preserve">"^http://data.europarl.europa.eu/reference/reds:.*$"</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">http://data.europarl.europa.eu/reference/reds:.*/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">entity$"</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">eponto:hasAgenda</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">http://data.europarl.europa.eu/reference/reds:.*/entity$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">eponto:hasAttendanceList</t>
@@ -685,7 +742,7 @@
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.58"/>
@@ -967,13 +1024,13 @@
   </sheetPr>
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="9" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="9" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.55"/>
@@ -1440,7 +1497,7 @@
       <c r="L24" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R24" s="14" t="s">
+      <c r="R24" s="0" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1464,8 +1521,8 @@
       <c r="L25" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R25" s="14" t="s">
-        <v>100</v>
+      <c r="R25" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,7 +1531,7 @@
         <v>epsh:P26</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>39</v>
@@ -1488,8 +1545,8 @@
       <c r="L26" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R26" s="14" t="s">
-        <v>100</v>
+      <c r="R26" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1498,7 +1555,7 @@
         <v>epsh:P27</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>39</v>
@@ -1512,8 +1569,8 @@
       <c r="L27" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R27" s="14" t="s">
-        <v>100</v>
+      <c r="R27" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1522,7 +1579,7 @@
         <v>epsh:P28</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>39</v>
@@ -1536,8 +1593,8 @@
       <c r="L28" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R28" s="14" t="s">
-        <v>100</v>
+      <c r="R28" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1546,7 +1603,7 @@
         <v>epsh:P29</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>39</v>
@@ -1557,8 +1614,8 @@
       <c r="L29" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R29" s="14" t="s">
-        <v>100</v>
+      <c r="R29" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1567,7 +1624,7 @@
         <v>epsh:P30</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>39</v>
@@ -1578,8 +1635,8 @@
       <c r="L30" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R30" s="14" t="s">
-        <v>100</v>
+      <c r="R30" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1588,7 +1645,7 @@
         <v>epsh:P31</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>39</v>
@@ -1602,8 +1659,8 @@
       <c r="L31" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R31" s="14" t="s">
-        <v>100</v>
+      <c r="R31" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1612,7 +1669,7 @@
         <v>epsh:P32</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>39</v>
@@ -1620,8 +1677,8 @@
       <c r="L32" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="R32" s="14" t="s">
-        <v>100</v>
+      <c r="R32" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1630,7 +1687,7 @@
         <v>epsh:P33</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>39</v>
@@ -1639,22 +1696,22 @@
         <v>35</v>
       </c>
       <c r="R33" s="14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="http://data.europarl.europa.eu/shapes"/>
     <hyperlink ref="E9" r:id="rId2" display="sh:name@fr"/>
-    <hyperlink ref="R24" r:id="rId3" display="&quot;^http://data.europarl.europa.eu/reference/reds:.*$&quot;"/>
-    <hyperlink ref="R25" r:id="rId4" display="&quot;^http://data.europarl.europa.eu/reference/reds:.*$&quot;"/>
-    <hyperlink ref="R26" r:id="rId5" display="&quot;^http://data.europarl.europa.eu/reference/reds:.*$&quot;"/>
-    <hyperlink ref="R27" r:id="rId6" display="&quot;^http://data.europarl.europa.eu/reference/reds:.*$&quot;"/>
-    <hyperlink ref="R28" r:id="rId7" display="&quot;^http://data.europarl.europa.eu/reference/reds:.*$&quot;"/>
-    <hyperlink ref="R29" r:id="rId8" display="&quot;^http://data.europarl.europa.eu/reference/reds:.*$&quot;"/>
-    <hyperlink ref="R30" r:id="rId9" display="&quot;^http://data.europarl.europa.eu/reference/reds:.*$&quot;"/>
-    <hyperlink ref="R31" r:id="rId10" display="&quot;^http://data.europarl.europa.eu/reference/reds:.*$&quot;"/>
-    <hyperlink ref="R32" r:id="rId11" display="&quot;^http://data.europarl.europa.eu/reference/reds:.*$&quot;"/>
+    <hyperlink ref="R24" r:id="rId3" display="http://data.europarl.europa.eu/reference/reds:.*/"/>
+    <hyperlink ref="R25" r:id="rId4" display="http://data.europarl.europa.eu/reference/reds:.*/entity$"/>
+    <hyperlink ref="R26" r:id="rId5" display="http://data.europarl.europa.eu/reference/reds:.*/entity$"/>
+    <hyperlink ref="R27" r:id="rId6" display="http://data.europarl.europa.eu/reference/reds:.*/entity$"/>
+    <hyperlink ref="R28" r:id="rId7" display="http://data.europarl.europa.eu/reference/reds:.*/entity$"/>
+    <hyperlink ref="R29" r:id="rId8" display="http://data.europarl.europa.eu/reference/reds:.*/entity$"/>
+    <hyperlink ref="R30" r:id="rId9" display="http://data.europarl.europa.eu/reference/reds:.*/entity$"/>
+    <hyperlink ref="R31" r:id="rId10" display="http://data.europarl.europa.eu/reference/reds:.*/entity$"/>
+    <hyperlink ref="R32" r:id="rId11" display="http://data.europarl.europa.eu/reference/reds:.*/entity$"/>
     <hyperlink ref="R33" r:id="rId12" display="&quot;^http://data.europarl.europa.eu/person/MEP_[0-9][0-9][0-9][0-9]?[0-9]?[0-9]?$&quot;"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>